<commit_message>
cleanup spreadsheets and remove old weatherfiles
</commit_message>
<xml_diff>
--- a/projects/office_calibration_rgenoud_14_Sys3.xlsx
+++ b/projects/office_calibration_rgenoud_14_Sys3.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$158</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$149</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2686" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2639" uniqueCount="864">
   <si>
     <t>type</t>
   </si>
@@ -2299,27 +2299,9 @@
     <t>Files to include (relative to this spreadsheet or absolute path). If a directory then it will include all subfolders and files</t>
   </si>
   <si>
-    <t>Calibrate South Window to Wall Ratio by Facade</t>
-  </si>
-  <si>
-    <t>South Window to Wall Ratio</t>
-  </si>
-  <si>
     <t>uniform_uncertain</t>
   </si>
   <si>
-    <t>Calibrate East Window to Wall Ratio by Facade</t>
-  </si>
-  <si>
-    <t>East Window to Wall Ratio</t>
-  </si>
-  <si>
-    <t>Calibrate West Window to Wall Ratio by Facade</t>
-  </si>
-  <si>
-    <t>West Window to Wall Ratio</t>
-  </si>
-  <si>
     <t>Lighting Power Reduction</t>
   </si>
   <si>
@@ -2639,6 +2621,18 @@
   </si>
   <si>
     <t>m2</t>
+  </si>
+  <si>
+    <t>Adjust Window to Wall Ratios</t>
+  </si>
+  <si>
+    <t>AdjustWindowToWallRatios</t>
+  </si>
+  <si>
+    <t>Window to Wall Ratio Multiplier</t>
+  </si>
+  <si>
+    <t>wwr_multiplier</t>
   </si>
 </sst>
 </file>
@@ -2831,7 +2825,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1836">
+  <cellStyleXfs count="1846">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4582,6 +4576,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4786,7 +4790,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1836">
+  <cellStyles count="1846">
     <cellStyle name="Comma" xfId="1749" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5705,6 +5709,11 @@
     <cellStyle name="Followed Hyperlink" xfId="1831" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1833" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1835" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1837" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1839" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1841" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1843" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1845" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6622,6 +6631,11 @@
     <cellStyle name="Hyperlink" xfId="1830" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1832" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1834" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1836" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1838" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1840" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1842" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1844" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7027,7 +7041,7 @@
         <v>470</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>472</v>
@@ -7098,7 +7112,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -7109,7 +7123,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>747</v>
@@ -7120,7 +7134,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>747</v>
@@ -7344,13 +7358,13 @@
     </row>
     <row r="35" spans="1:5" s="31" customFormat="1">
       <c r="A35" s="31" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="B35" s="30">
         <v>1</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="D35" s="2"/>
     </row>
@@ -7427,7 +7441,7 @@
         <v>699</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1">
@@ -7458,11 +7472,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y231"/>
+  <dimension ref="A1:Y222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7478,7 +7492,7 @@
     <col min="9" max="9" width="8.6640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="7.1640625" style="31" customWidth="1"/>
     <col min="11" max="11" width="8.1640625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" style="31" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="7.6640625" style="31" customWidth="1"/>
     <col min="15" max="15" width="11.5" style="31"/>
     <col min="16" max="16" width="11.5" style="31" customWidth="1"/>
@@ -7726,7 +7740,7 @@
         <v>618</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -7864,7 +7878,7 @@
         <v>0.25</v>
       </c>
       <c r="Q15" s="50" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="16" spans="1:25" s="30" customFormat="1">
@@ -7920,7 +7934,7 @@
         <v>0.5</v>
       </c>
       <c r="Q17" s="50" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="30" customFormat="1">
@@ -8184,13 +8198,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="E33" s="37" t="s">
         <v>68</v>
@@ -8203,10 +8217,10 @@
         <v>22</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="F34" s="42" t="s">
         <v>64</v>
@@ -8231,7 +8245,7 @@
         <v>0.05</v>
       </c>
       <c r="Q34" s="42" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="42" customFormat="1">
@@ -8239,10 +8253,10 @@
         <v>22</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="F35" s="42" t="s">
         <v>64</v>
@@ -8267,7 +8281,7 @@
         <v>0.05</v>
       </c>
       <c r="Q35" s="42" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="36" spans="1:17" s="37" customFormat="1">
@@ -8275,7 +8289,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="C36" s="37" t="s">
         <v>74</v>
@@ -8294,7 +8308,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="E37" s="42" t="s">
         <v>75</v>
@@ -8303,7 +8317,7 @@
         <v>619</v>
       </c>
       <c r="G37" s="42" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="H37" s="42">
         <v>0</v>
@@ -8325,7 +8339,7 @@
         <v>5</v>
       </c>
       <c r="Q37" s="42" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="37" customFormat="1">
@@ -8364,26 +8378,10 @@
         <v>0.4</v>
       </c>
       <c r="I39" s="3"/>
-      <c r="J39" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K39" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="L39" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="M39" s="31">
-        <f>(K39-J39)/6</f>
-        <v>0.125</v>
-      </c>
-      <c r="N39" s="31">
-        <v>0.01</v>
-      </c>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
       <c r="P39" s="39"/>
-      <c r="Q39" s="31" t="s">
-        <v>754</v>
-      </c>
     </row>
     <row r="40" spans="1:17">
       <c r="B40" s="31" t="s">
@@ -8471,26 +8469,10 @@
         <v>0.4</v>
       </c>
       <c r="I43" s="3"/>
-      <c r="J43" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K43" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="L43" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="M43" s="31">
-        <f>(K43-J43)/6</f>
-        <v>0.125</v>
-      </c>
-      <c r="N43" s="31">
-        <v>0.01</v>
-      </c>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
       <c r="P43" s="39"/>
-      <c r="Q43" s="31" t="s">
-        <v>754</v>
-      </c>
     </row>
     <row r="44" spans="1:17">
       <c r="B44" s="31" t="s">
@@ -8578,26 +8560,10 @@
         <v>0.4</v>
       </c>
       <c r="I47" s="3"/>
-      <c r="J47" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K47" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="L47" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="M47" s="31">
-        <f>(K47-J47)/6</f>
-        <v>0.125</v>
-      </c>
-      <c r="N47" s="31">
-        <v>0.01</v>
-      </c>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
       <c r="P47" s="39"/>
-      <c r="Q47" s="31" t="s">
-        <v>754</v>
-      </c>
     </row>
     <row r="48" spans="1:17">
       <c r="B48" s="31" t="s">
@@ -8685,26 +8651,10 @@
         <v>0.4</v>
       </c>
       <c r="I51" s="3"/>
-      <c r="J51" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="K51" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="L51" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="M51" s="31">
-        <f>(K51-J51)/6</f>
-        <v>0.125</v>
-      </c>
-      <c r="N51" s="31">
-        <v>0.01</v>
-      </c>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
       <c r="P51" s="39"/>
-      <c r="Q51" s="31" t="s">
-        <v>754</v>
-      </c>
     </row>
     <row r="52" spans="1:17">
       <c r="B52" s="31" t="s">
@@ -8825,7 +8775,7 @@
         <v>618</v>
       </c>
       <c r="H57" s="40" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="I57" s="31"/>
     </row>
@@ -8843,7 +8793,7 @@
         <v>618</v>
       </c>
       <c r="H58" s="40" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="I58" s="31"/>
     </row>
@@ -8852,13 +8802,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="C59" s="37" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="D59" s="37" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="E59" s="37" t="s">
         <v>68</v>
@@ -8871,16 +8821,16 @@
         <v>21</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>810</v>
+        <v>804</v>
       </c>
       <c r="E60" s="31" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="F60" s="31" t="s">
         <v>618</v>
       </c>
       <c r="H60" s="31" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="I60" s="31"/>
     </row>
@@ -8889,16 +8839,16 @@
         <v>22</v>
       </c>
       <c r="D61" s="42" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="E61" s="42" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="F61" s="42" t="s">
         <v>619</v>
       </c>
       <c r="G61" s="42" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="H61" s="42">
         <v>1</v>
@@ -8921,7 +8871,7 @@
       </c>
       <c r="P61" s="46"/>
       <c r="Q61" s="42" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="37" customFormat="1">
@@ -8948,13 +8898,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="48" t="s">
-        <v>752</v>
+        <v>860</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>76</v>
+        <v>861</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>76</v>
+        <v>861</v>
       </c>
       <c r="E63" s="48" t="s">
         <v>68</v>
@@ -8965,35 +8915,39 @@
         <v>22</v>
       </c>
       <c r="D64" s="42" t="s">
-        <v>753</v>
+        <v>862</v>
       </c>
       <c r="E64" s="42" t="s">
-        <v>77</v>
+        <v>863</v>
       </c>
       <c r="F64" s="42" t="s">
         <v>64</v>
       </c>
       <c r="H64" s="42">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="J64" s="42">
+        <f>0.05/H47</f>
+        <v>0.125</v>
+      </c>
+      <c r="K64" s="42">
+        <f>0.8/H43</f>
+        <v>2</v>
+      </c>
+      <c r="L64" s="42">
+        <f>AVERAGE(J64:K64)</f>
+        <v>1.0625</v>
+      </c>
+      <c r="M64" s="42">
+        <f>(K64-J64)/6</f>
+        <v>0.3125</v>
+      </c>
+      <c r="N64" s="42">
+        <f>0.05</f>
         <v>0.05</v>
       </c>
-      <c r="K64" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="L64" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="M64" s="42">
-        <f>(K64+J64)/6</f>
-        <v>0.14166666666666669</v>
-      </c>
-      <c r="N64" s="42">
-        <v>0.05</v>
-      </c>
       <c r="Q64" s="42" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="65" spans="1:17" s="30" customFormat="1">
@@ -9001,7 +8955,7 @@
         <v>21</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>78</v>
+        <v>666</v>
       </c>
       <c r="E65" s="30" t="s">
         <v>79</v>
@@ -9009,81 +8963,85 @@
       <c r="F65" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G65" s="30" t="s">
+        <v>667</v>
+      </c>
       <c r="H65" s="30">
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="30" customFormat="1">
-      <c r="B66" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D66" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E66" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F66" s="30" t="s">
+    <row r="66" spans="1:17" s="48" customFormat="1">
+      <c r="A66" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="B66" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" s="30" customFormat="1">
+      <c r="B67" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F67" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H66" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="I66" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" s="48" customFormat="1">
-      <c r="A67" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="B67" s="48" t="s">
-        <v>755</v>
-      </c>
-      <c r="C67" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="D67" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="E67" s="48" t="s">
-        <v>68</v>
-      </c>
+      <c r="H67" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I67" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="O67" s="31"/>
     </row>
     <row r="68" spans="1:17" s="42" customFormat="1">
       <c r="B68" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D68" s="42" t="s">
-        <v>756</v>
+      <c r="D68" s="43" t="s">
+        <v>818</v>
       </c>
       <c r="E68" s="42" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F68" s="42" t="s">
         <v>64</v>
       </c>
       <c r="H68" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="J68" s="42">
-        <v>0.05</v>
-      </c>
-      <c r="K68" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="L68" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="M68" s="42">
-        <f>(K68+J68)/6</f>
-        <v>0.14166666666666669</v>
-      </c>
-      <c r="N68" s="42">
-        <v>0.05</v>
+        <v>0</v>
+      </c>
+      <c r="J68" s="44">
+        <v>-100</v>
+      </c>
+      <c r="K68" s="44">
+        <v>100</v>
+      </c>
+      <c r="L68" s="44">
+        <v>0</v>
+      </c>
+      <c r="M68" s="44">
+        <f>(K68-J68)/6</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="N68" s="44">
+        <v>2.5</v>
       </c>
       <c r="Q68" s="42" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="30" customFormat="1">
@@ -9091,89 +9049,86 @@
         <v>21</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>78</v>
+        <v>810</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>79</v>
+        <v>811</v>
       </c>
       <c r="F69" s="30" t="s">
         <v>64</v>
       </c>
       <c r="H69" s="30">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" s="30" customFormat="1">
-      <c r="B70" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D70" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E70" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F70" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H70" s="30" t="s">
-        <v>669</v>
-      </c>
-      <c r="I70" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" s="48" customFormat="1">
-      <c r="A71" s="48" t="b">
         <v>1</v>
       </c>
-      <c r="B71" s="48" t="s">
-        <v>757</v>
-      </c>
-      <c r="C71" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="D71" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="E71" s="48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" s="42" customFormat="1">
-      <c r="B72" s="42" t="s">
+    </row>
+    <row r="70" spans="1:17" s="42" customFormat="1">
+      <c r="B70" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D72" s="42" t="s">
-        <v>758</v>
-      </c>
-      <c r="E72" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="F72" s="42" t="s">
+      <c r="D70" s="43" t="s">
+        <v>813</v>
+      </c>
+      <c r="E70" s="42" t="s">
+        <v>812</v>
+      </c>
+      <c r="F70" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="H72" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="J72" s="42">
+      <c r="H70" s="42">
+        <v>0</v>
+      </c>
+      <c r="J70" s="44">
+        <v>0</v>
+      </c>
+      <c r="K70" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="L70" s="44">
         <v>0.05</v>
       </c>
-      <c r="K72" s="42">
-        <v>0.8</v>
-      </c>
-      <c r="L72" s="42">
-        <v>0.4</v>
-      </c>
-      <c r="M72" s="42">
-        <f>(K72+J72)/6</f>
-        <v>0.14166666666666669</v>
-      </c>
-      <c r="N72" s="42">
-        <v>0.05</v>
-      </c>
-      <c r="Q72" s="42" t="s">
-        <v>754</v>
+      <c r="M70" s="44">
+        <f>(K70-J70)/6</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="N70" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="Q70" s="42" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" s="30" customFormat="1">
+      <c r="B71" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>815</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>814</v>
+      </c>
+      <c r="F71" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H71" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="30" customFormat="1">
+      <c r="B72" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>817</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>816</v>
+      </c>
+      <c r="F72" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H72" s="30">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="30" customFormat="1">
@@ -9181,16 +9136,16 @@
         <v>21</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="F73" s="30" t="s">
         <v>64</v>
       </c>
       <c r="H73" s="30">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="30" customFormat="1">
@@ -9198,726 +9153,722 @@
         <v>21</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="F74" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H74" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" s="30" customFormat="1">
+      <c r="B75" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E75" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F75" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H75" s="30">
+        <v>1</v>
+      </c>
+      <c r="O75" s="31"/>
+    </row>
+    <row r="76" spans="1:17" s="49" customFormat="1">
+      <c r="A76" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B76" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C76" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E76" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17">
+      <c r="A77" s="30"/>
+      <c r="B77" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H74" s="30" t="s">
-        <v>670</v>
-      </c>
-      <c r="I74" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" s="48" customFormat="1">
-      <c r="A75" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="B75" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="C75" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="D75" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="E75" s="48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" s="30" customFormat="1">
-      <c r="B76" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D76" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F76" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H76" s="30" t="s">
+      <c r="G77" s="30"/>
+      <c r="H77" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I76" s="30" t="s">
+      <c r="I77" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="O76" s="31"/>
-    </row>
-    <row r="77" spans="1:17" s="42" customFormat="1">
-      <c r="B77" s="42" t="s">
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="P77" s="39"/>
+    </row>
+    <row r="78" spans="1:17" s="42" customFormat="1">
+      <c r="B78" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D77" s="43" t="s">
-        <v>824</v>
-      </c>
-      <c r="E77" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="F77" s="42" t="s">
+      <c r="D78" s="42" t="s">
+        <v>753</v>
+      </c>
+      <c r="E78" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="H77" s="42">
-        <v>0</v>
-      </c>
-      <c r="J77" s="44">
-        <v>-100</v>
-      </c>
-      <c r="K77" s="44">
-        <v>100</v>
-      </c>
-      <c r="L77" s="44">
-        <v>0</v>
-      </c>
-      <c r="M77" s="44">
-        <f>(K77-J77)/6</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="N77" s="44">
+      <c r="H78" s="42">
+        <v>0</v>
+      </c>
+      <c r="I78" s="45"/>
+      <c r="J78" s="44">
+        <v>-60</v>
+      </c>
+      <c r="K78" s="44">
+        <v>60</v>
+      </c>
+      <c r="L78" s="44">
+        <v>-1</v>
+      </c>
+      <c r="M78" s="44">
+        <f>(K78-J78)/6</f>
+        <v>20</v>
+      </c>
+      <c r="N78" s="44">
         <v>2.5</v>
       </c>
-      <c r="Q77" s="42" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" s="30" customFormat="1">
-      <c r="B78" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" s="30" t="s">
-        <v>816</v>
-      </c>
-      <c r="E78" s="30" t="s">
-        <v>817</v>
-      </c>
-      <c r="F78" s="30" t="s">
+      <c r="P78" s="46"/>
+      <c r="Q78" s="42" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17">
+      <c r="A79" s="30"/>
+      <c r="B79" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79" s="30"/>
+      <c r="D79" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F79" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H78" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" s="42" customFormat="1">
-      <c r="B79" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D79" s="43" t="s">
-        <v>819</v>
-      </c>
-      <c r="E79" s="42" t="s">
-        <v>818</v>
-      </c>
-      <c r="F79" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="H79" s="42">
-        <v>0</v>
-      </c>
-      <c r="J79" s="44">
-        <v>0</v>
-      </c>
-      <c r="K79" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="L79" s="44">
-        <v>0.05</v>
-      </c>
-      <c r="M79" s="44">
-        <f>(K79-J79)/6</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="N79" s="44">
-        <v>0.01</v>
-      </c>
-      <c r="Q79" s="42" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" s="30" customFormat="1">
+      <c r="G79" s="30"/>
+      <c r="H79" s="30">
+        <v>0</v>
+      </c>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="P79" s="39"/>
+    </row>
+    <row r="80" spans="1:17">
+      <c r="A80" s="30"/>
       <c r="B80" s="30" t="s">
         <v>21</v>
       </c>
+      <c r="C80" s="30"/>
       <c r="D80" s="30" t="s">
-        <v>821</v>
+        <v>49</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>820</v>
+        <v>50</v>
       </c>
       <c r="F80" s="30" t="s">
         <v>64</v>
       </c>
+      <c r="G80" s="30"/>
       <c r="H80" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:17" s="30" customFormat="1">
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="P80" s="39"/>
+    </row>
+    <row r="81" spans="1:17">
+      <c r="A81" s="30"/>
       <c r="B81" s="30" t="s">
         <v>21</v>
       </c>
+      <c r="C81" s="30"/>
       <c r="D81" s="30" t="s">
-        <v>823</v>
+        <v>51</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>822</v>
+        <v>52</v>
       </c>
       <c r="F81" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G81" s="30"/>
+      <c r="H81" s="30">
+        <v>0</v>
+      </c>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="P81" s="39"/>
+    </row>
+    <row r="82" spans="1:17">
+      <c r="A82" s="30"/>
+      <c r="B82" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F82" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G82" s="30"/>
+      <c r="H82" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="P82" s="39"/>
+    </row>
+    <row r="83" spans="1:17">
+      <c r="A83" s="30"/>
+      <c r="B83" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F83" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G83" s="30"/>
+      <c r="H83" s="30">
+        <v>15</v>
+      </c>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="P83" s="39"/>
+    </row>
+    <row r="84" spans="1:17">
+      <c r="A84" s="30"/>
+      <c r="B84" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F84" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H81" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" s="30" customFormat="1">
-      <c r="B82" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E82" s="30" t="s">
+      <c r="G84" s="30"/>
+      <c r="H84" s="30">
+        <v>0</v>
+      </c>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="P84" s="39"/>
+    </row>
+    <row r="85" spans="1:17">
+      <c r="A85" s="30"/>
+      <c r="B85" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F85" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G85" s="30"/>
+      <c r="H85" s="30">
+        <v>1</v>
+      </c>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="P85" s="39"/>
+    </row>
+    <row r="86" spans="1:17" s="49" customFormat="1">
+      <c r="A86" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B86" s="49" t="s">
+        <v>327</v>
+      </c>
+      <c r="C86" s="49" t="s">
+        <v>328</v>
+      </c>
+      <c r="D86" s="49" t="s">
+        <v>328</v>
+      </c>
+      <c r="E86" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17">
+      <c r="A87" s="30"/>
+      <c r="B87" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="E87" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G87" s="30"/>
+      <c r="H87" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I87" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="P87" s="39"/>
+    </row>
+    <row r="88" spans="1:17" s="42" customFormat="1">
+      <c r="B88" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D88" s="42" t="s">
+        <v>769</v>
+      </c>
+      <c r="E88" s="42" t="s">
+        <v>330</v>
+      </c>
+      <c r="F88" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H88" s="42">
+        <v>0</v>
+      </c>
+      <c r="I88" s="45"/>
+      <c r="J88" s="44">
+        <v>-30</v>
+      </c>
+      <c r="K88" s="44">
+        <v>30</v>
+      </c>
+      <c r="L88" s="44">
+        <v>0</v>
+      </c>
+      <c r="M88" s="44">
+        <f>(K88-J88)/6</f>
+        <v>10</v>
+      </c>
+      <c r="N88" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q88" s="42" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" s="49" customFormat="1">
+      <c r="A89" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B89" s="49" t="s">
+        <v>770</v>
+      </c>
+      <c r="C89" s="49" t="s">
+        <v>771</v>
+      </c>
+      <c r="D89" s="49" t="s">
+        <v>771</v>
+      </c>
+      <c r="E89" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" s="42" customFormat="1">
+      <c r="B90" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90" s="42" t="s">
+        <v>772</v>
+      </c>
+      <c r="E90" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="F90" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H90" s="42">
+        <v>0</v>
+      </c>
+      <c r="I90" s="45"/>
+      <c r="J90" s="44">
+        <v>-50</v>
+      </c>
+      <c r="K90" s="44">
+        <v>200</v>
+      </c>
+      <c r="L90" s="44">
+        <v>0</v>
+      </c>
+      <c r="M90" s="44">
+        <f>(K90-J90)/6</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="N90" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q90" s="42" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="49" customFormat="1">
+      <c r="A91" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B91" s="49" t="s">
+        <v>773</v>
+      </c>
+      <c r="C91" s="49" t="s">
+        <v>774</v>
+      </c>
+      <c r="D91" s="49" t="s">
+        <v>774</v>
+      </c>
+      <c r="E91" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" s="42" customFormat="1">
+      <c r="B92" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" s="42" t="s">
+        <v>775</v>
+      </c>
+      <c r="E92" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="F92" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H92" s="42">
+        <v>0</v>
+      </c>
+      <c r="I92" s="45"/>
+      <c r="J92" s="44">
+        <v>-50</v>
+      </c>
+      <c r="K92" s="44">
+        <v>100</v>
+      </c>
+      <c r="L92" s="44">
+        <v>0</v>
+      </c>
+      <c r="M92" s="44">
+        <f>(K92-J92)/6</f>
+        <v>25</v>
+      </c>
+      <c r="N92" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q92" s="42" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" s="49" customFormat="1">
+      <c r="A93" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B93" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="C93" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="D93" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="E93" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" s="30" customFormat="1">
+      <c r="B94" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="E94" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F94" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H94" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I94" s="30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" s="42" customFormat="1">
+      <c r="B95" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>776</v>
+      </c>
+      <c r="E95" s="42" t="s">
+        <v>288</v>
+      </c>
+      <c r="F95" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="G95" s="42" t="s">
+        <v>777</v>
+      </c>
+      <c r="H95" s="42">
+        <v>0</v>
+      </c>
+      <c r="I95" s="45"/>
+      <c r="J95" s="44">
+        <v>-80</v>
+      </c>
+      <c r="K95" s="44">
+        <v>80</v>
+      </c>
+      <c r="L95" s="44">
+        <v>-1</v>
+      </c>
+      <c r="M95" s="44">
+        <f>(K95-J95)/6</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="N95" s="44">
+        <v>2.5</v>
+      </c>
+      <c r="Q95" s="42" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" s="30" customFormat="1">
+      <c r="B96" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D96" s="30" t="s">
+        <v>778</v>
+      </c>
+      <c r="E96" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F82" s="30" t="s">
+      <c r="F96" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H82" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" s="30" customFormat="1">
-      <c r="B83" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D83" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E83" s="30" t="s">
+      <c r="G96" s="30" t="s">
+        <v>777</v>
+      </c>
+      <c r="H96" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" s="30" customFormat="1">
+      <c r="B97" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D97" s="30" t="s">
+        <v>779</v>
+      </c>
+      <c r="E97" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F97" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G97" s="30" t="s">
+        <v>777</v>
+      </c>
+      <c r="H97" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" s="30" customFormat="1">
+      <c r="B98" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>780</v>
+      </c>
+      <c r="E98" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F98" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G98" s="30" t="s">
+        <v>781</v>
+      </c>
+      <c r="H98" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" s="30" customFormat="1">
+      <c r="B99" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>782</v>
+      </c>
+      <c r="E99" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F99" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H99" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" s="30" customFormat="1">
+      <c r="B100" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>783</v>
+      </c>
+      <c r="E100" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F100" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G100" s="30" t="s">
+        <v>781</v>
+      </c>
+      <c r="H100" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" s="30" customFormat="1">
+      <c r="B101" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="30" t="s">
+        <v>784</v>
+      </c>
+      <c r="E101" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F83" s="30" t="s">
+      <c r="F101" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H83" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" s="30" customFormat="1">
-      <c r="B84" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D84" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E84" s="30" t="s">
+      <c r="G101" s="30" t="s">
+        <v>777</v>
+      </c>
+      <c r="H101" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" s="30" customFormat="1">
+      <c r="B102" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102" s="30" t="s">
+        <v>785</v>
+      </c>
+      <c r="E102" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F84" s="30" t="s">
+      <c r="F102" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="H84" s="30">
+      <c r="G102" s="30" t="s">
+        <v>781</v>
+      </c>
+      <c r="H102" s="30">
         <v>1</v>
       </c>
-      <c r="O84" s="31"/>
-    </row>
-    <row r="85" spans="1:17" s="49" customFormat="1">
-      <c r="A85" s="49" t="b">
+    </row>
+    <row r="103" spans="1:17" s="49" customFormat="1">
+      <c r="A103" s="49" t="b">
         <v>1</v>
       </c>
-      <c r="B85" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C85" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="D85" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="E85" s="49" t="s">
+      <c r="B103" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C103" s="49" t="s">
+        <v>794</v>
+      </c>
+      <c r="D103" s="49" t="s">
+        <v>794</v>
+      </c>
+      <c r="E103" s="49" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E86" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F86" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G86" s="30"/>
-      <c r="H86" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I86" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
-      <c r="M86" s="3"/>
-      <c r="N86" s="3"/>
-      <c r="P86" s="39"/>
-    </row>
-    <row r="87" spans="1:17" s="42" customFormat="1">
-      <c r="B87" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D87" s="42" t="s">
-        <v>759</v>
-      </c>
-      <c r="E87" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F87" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="H87" s="42">
-        <v>0</v>
-      </c>
-      <c r="I87" s="45"/>
-      <c r="J87" s="44">
-        <v>-60</v>
-      </c>
-      <c r="K87" s="44">
-        <v>60</v>
-      </c>
-      <c r="L87" s="44">
-        <v>-1</v>
-      </c>
-      <c r="M87" s="44">
-        <f>(K87-J87)/6</f>
-        <v>20</v>
-      </c>
-      <c r="N87" s="44">
-        <v>2.5</v>
-      </c>
-      <c r="P87" s="46"/>
-      <c r="Q87" s="42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C88" s="30"/>
-      <c r="D88" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="E88" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F88" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G88" s="30"/>
-      <c r="H88" s="30">
-        <v>0</v>
-      </c>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
-      <c r="N88" s="3"/>
-      <c r="P88" s="39"/>
-    </row>
-    <row r="89" spans="1:17">
-      <c r="A89" s="30"/>
-      <c r="B89" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E89" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F89" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G89" s="30"/>
-      <c r="H89" s="30">
-        <v>0</v>
-      </c>
-      <c r="J89" s="3"/>
-      <c r="K89" s="3"/>
-      <c r="L89" s="3"/>
-      <c r="M89" s="3"/>
-      <c r="N89" s="3"/>
-      <c r="P89" s="39"/>
-    </row>
-    <row r="90" spans="1:17">
-      <c r="A90" s="30"/>
-      <c r="B90" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E90" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F90" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G90" s="30"/>
-      <c r="H90" s="30">
-        <v>0</v>
-      </c>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="3"/>
-      <c r="P90" s="39"/>
-    </row>
-    <row r="91" spans="1:17">
-      <c r="A91" s="30"/>
-      <c r="B91" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E91" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F91" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G91" s="30"/>
-      <c r="H91" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J91" s="3"/>
-      <c r="K91" s="3"/>
-      <c r="L91" s="3"/>
-      <c r="M91" s="3"/>
-      <c r="N91" s="3"/>
-      <c r="P91" s="39"/>
-    </row>
-    <row r="92" spans="1:17">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E92" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="F92" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G92" s="30"/>
-      <c r="H92" s="30">
-        <v>15</v>
-      </c>
-      <c r="J92" s="3"/>
-      <c r="K92" s="3"/>
-      <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
-      <c r="N92" s="3"/>
-      <c r="P92" s="39"/>
-    </row>
-    <row r="93" spans="1:17">
-      <c r="A93" s="30"/>
-      <c r="B93" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="E93" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F93" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G93" s="30"/>
-      <c r="H93" s="30">
-        <v>0</v>
-      </c>
-      <c r="J93" s="3"/>
-      <c r="K93" s="3"/>
-      <c r="L93" s="3"/>
-      <c r="M93" s="3"/>
-      <c r="N93" s="3"/>
-      <c r="P93" s="39"/>
-    </row>
-    <row r="94" spans="1:17">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E94" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F94" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G94" s="30"/>
-      <c r="H94" s="30">
-        <v>1</v>
-      </c>
-      <c r="J94" s="3"/>
-      <c r="K94" s="3"/>
-      <c r="L94" s="3"/>
-      <c r="M94" s="3"/>
-      <c r="N94" s="3"/>
-      <c r="P94" s="39"/>
-    </row>
-    <row r="95" spans="1:17" s="49" customFormat="1">
-      <c r="A95" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B95" s="49" t="s">
-        <v>327</v>
-      </c>
-      <c r="C95" s="49" t="s">
-        <v>328</v>
-      </c>
-      <c r="D95" s="49" t="s">
-        <v>328</v>
-      </c>
-      <c r="E95" s="49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17">
-      <c r="A96" s="30"/>
-      <c r="B96" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30" t="s">
-        <v>373</v>
-      </c>
-      <c r="E96" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F96" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G96" s="30"/>
-      <c r="H96" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I96" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
-      <c r="P96" s="39"/>
-    </row>
-    <row r="97" spans="1:17" s="42" customFormat="1">
-      <c r="B97" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D97" s="42" t="s">
-        <v>775</v>
-      </c>
-      <c r="E97" s="42" t="s">
-        <v>330</v>
-      </c>
-      <c r="F97" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="H97" s="42">
-        <v>0</v>
-      </c>
-      <c r="I97" s="45"/>
-      <c r="J97" s="44">
-        <v>-30</v>
-      </c>
-      <c r="K97" s="44">
-        <v>30</v>
-      </c>
-      <c r="L97" s="44">
-        <v>0</v>
-      </c>
-      <c r="M97" s="44">
-        <f>(K97-J97)/6</f>
-        <v>10</v>
-      </c>
-      <c r="N97" s="44">
-        <v>2.5</v>
-      </c>
-      <c r="Q97" s="42" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17" s="49" customFormat="1">
-      <c r="A98" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B98" s="49" t="s">
-        <v>776</v>
-      </c>
-      <c r="C98" s="49" t="s">
-        <v>777</v>
-      </c>
-      <c r="D98" s="49" t="s">
-        <v>777</v>
-      </c>
-      <c r="E98" s="49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" s="42" customFormat="1">
-      <c r="B99" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D99" s="42" t="s">
-        <v>778</v>
-      </c>
-      <c r="E99" s="42" t="s">
-        <v>258</v>
-      </c>
-      <c r="F99" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="H99" s="42">
-        <v>0</v>
-      </c>
-      <c r="I99" s="45"/>
-      <c r="J99" s="44">
-        <v>-50</v>
-      </c>
-      <c r="K99" s="44">
-        <v>200</v>
-      </c>
-      <c r="L99" s="44">
-        <v>0</v>
-      </c>
-      <c r="M99" s="44">
-        <f>(K99-J99)/6</f>
-        <v>41.666666666666664</v>
-      </c>
-      <c r="N99" s="44">
-        <v>2.5</v>
-      </c>
-      <c r="Q99" s="42" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" s="49" customFormat="1">
-      <c r="A100" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B100" s="49" t="s">
-        <v>779</v>
-      </c>
-      <c r="C100" s="49" t="s">
-        <v>780</v>
-      </c>
-      <c r="D100" s="49" t="s">
-        <v>780</v>
-      </c>
-      <c r="E100" s="49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="101" spans="1:17" s="42" customFormat="1">
-      <c r="B101" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D101" s="42" t="s">
-        <v>781</v>
-      </c>
-      <c r="E101" s="42" t="s">
-        <v>258</v>
-      </c>
-      <c r="F101" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="H101" s="42">
-        <v>0</v>
-      </c>
-      <c r="I101" s="45"/>
-      <c r="J101" s="44">
-        <v>-50</v>
-      </c>
-      <c r="K101" s="44">
-        <v>100</v>
-      </c>
-      <c r="L101" s="44">
-        <v>0</v>
-      </c>
-      <c r="M101" s="44">
-        <f>(K101-J101)/6</f>
-        <v>25</v>
-      </c>
-      <c r="N101" s="44">
-        <v>2.5</v>
-      </c>
-      <c r="Q101" s="42" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17" s="49" customFormat="1">
-      <c r="A102" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B102" s="49" t="s">
-        <v>285</v>
-      </c>
-      <c r="C102" s="49" t="s">
-        <v>286</v>
-      </c>
-      <c r="D102" s="49" t="s">
-        <v>286</v>
-      </c>
-      <c r="E102" s="49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" s="30" customFormat="1">
-      <c r="B103" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D103" s="30" t="s">
-        <v>373</v>
-      </c>
-      <c r="E103" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F103" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H103" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I103" s="30" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:17" s="42" customFormat="1">
@@ -9925,348 +9876,188 @@
         <v>22</v>
       </c>
       <c r="D104" s="42" t="s">
-        <v>782</v>
+        <v>795</v>
       </c>
       <c r="E104" s="42" t="s">
-        <v>288</v>
+        <v>190</v>
       </c>
       <c r="F104" s="42" t="s">
         <v>64</v>
       </c>
       <c r="G104" s="42" t="s">
-        <v>783</v>
+        <v>796</v>
       </c>
       <c r="H104" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104" s="45"/>
       <c r="J104" s="44">
-        <v>-80</v>
+        <v>-2</v>
       </c>
       <c r="K104" s="44">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="L104" s="44">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M104" s="44">
         <f>(K104-J104)/6</f>
-        <v>26.666666666666668</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N104" s="44">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="Q104" s="42" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" s="30" customFormat="1">
-      <c r="B105" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D105" s="30" t="s">
-        <v>784</v>
-      </c>
-      <c r="E105" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F105" s="30" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" s="42" customFormat="1">
+      <c r="B105" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D105" s="42" t="s">
+        <v>797</v>
+      </c>
+      <c r="E105" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="F105" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="G105" s="30" t="s">
-        <v>783</v>
-      </c>
-      <c r="H105" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" s="30" customFormat="1">
-      <c r="B106" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D106" s="30" t="s">
-        <v>785</v>
-      </c>
-      <c r="E106" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="F106" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G106" s="30" t="s">
-        <v>783</v>
-      </c>
-      <c r="H106" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:17" s="30" customFormat="1">
-      <c r="B107" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D107" s="30" t="s">
-        <v>786</v>
-      </c>
-      <c r="E107" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F107" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G107" s="30" t="s">
-        <v>787</v>
-      </c>
-      <c r="H107" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:17" s="30" customFormat="1">
-      <c r="B108" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D108" s="30" t="s">
-        <v>788</v>
-      </c>
-      <c r="E108" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F108" s="30" t="s">
+      <c r="G105" s="42" t="s">
+        <v>796</v>
+      </c>
+      <c r="H105" s="42">
+        <v>-1</v>
+      </c>
+      <c r="I105" s="45"/>
+      <c r="J105" s="44">
+        <v>-2</v>
+      </c>
+      <c r="K105" s="44">
+        <v>2</v>
+      </c>
+      <c r="L105" s="44">
+        <v>0</v>
+      </c>
+      <c r="M105" s="44">
+        <f>(K105-J105)/6</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="N105" s="44">
+        <v>1</v>
+      </c>
+      <c r="Q105" s="42" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17">
+      <c r="B106" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106" s="31" t="s">
+        <v>798</v>
+      </c>
+      <c r="E106" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="F106" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="H108" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:17" s="30" customFormat="1">
-      <c r="B109" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D109" s="30" t="s">
-        <v>789</v>
-      </c>
-      <c r="E109" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="F109" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G109" s="30" t="s">
-        <v>787</v>
-      </c>
-      <c r="H109" s="30">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="110" spans="1:17" s="30" customFormat="1">
-      <c r="B110" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D110" s="30" t="s">
-        <v>790</v>
-      </c>
-      <c r="E110" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F110" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G110" s="30" t="s">
-        <v>783</v>
-      </c>
-      <c r="H110" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:17" s="30" customFormat="1">
-      <c r="B111" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D111" s="30" t="s">
-        <v>791</v>
-      </c>
-      <c r="E111" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="F111" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G111" s="30" t="s">
-        <v>787</v>
-      </c>
-      <c r="H111" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:17" s="37" customFormat="1">
-      <c r="A112" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="B112" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="C112" s="37" t="s">
-        <v>800</v>
-      </c>
-      <c r="D112" s="37" t="s">
-        <v>800</v>
-      </c>
-      <c r="E112" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G112" s="38"/>
-      <c r="H112" s="38"/>
-    </row>
-    <row r="113" spans="2:17" s="42" customFormat="1">
-      <c r="B113" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D113" s="42" t="s">
-        <v>801</v>
-      </c>
-      <c r="E113" s="42" t="s">
-        <v>190</v>
-      </c>
-      <c r="F113" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G113" s="42" t="s">
-        <v>802</v>
-      </c>
-      <c r="H113" s="42">
-        <v>1</v>
-      </c>
-      <c r="I113" s="45"/>
-      <c r="J113" s="44">
-        <v>-2</v>
-      </c>
-      <c r="K113" s="44">
-        <v>2</v>
-      </c>
-      <c r="L113" s="44">
-        <v>0</v>
-      </c>
-      <c r="M113" s="44">
-        <f>(K113-J113)/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="N113" s="44">
-        <v>1</v>
-      </c>
-      <c r="Q113" s="42" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="114" spans="2:17" s="42" customFormat="1">
-      <c r="B114" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="D114" s="42" t="s">
-        <v>803</v>
-      </c>
-      <c r="E114" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="F114" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="G114" s="42" t="s">
-        <v>802</v>
-      </c>
-      <c r="H114" s="42">
-        <v>-1</v>
-      </c>
-      <c r="I114" s="45"/>
-      <c r="J114" s="44">
-        <v>-2</v>
-      </c>
-      <c r="K114" s="44">
-        <v>2</v>
-      </c>
-      <c r="L114" s="44">
-        <v>0</v>
-      </c>
-      <c r="M114" s="44">
-        <f>(K114-J114)/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="N114" s="44">
-        <v>1</v>
-      </c>
-      <c r="Q114" s="42" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="115" spans="2:17">
-      <c r="B115" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D115" s="31" t="s">
-        <v>804</v>
-      </c>
-      <c r="E115" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="F115" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="H115" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J115" s="3"/>
-      <c r="K115" s="3"/>
-      <c r="L115" s="3"/>
-      <c r="M115" s="3"/>
-      <c r="N115" s="3"/>
-    </row>
-    <row r="116" spans="2:17">
+      <c r="H106" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+    </row>
+    <row r="107" spans="1:17">
+      <c r="H107" s="31"/>
+      <c r="I107" s="31"/>
+    </row>
+    <row r="108" spans="1:17">
+      <c r="H108" s="31"/>
+      <c r="I108" s="31"/>
+    </row>
+    <row r="109" spans="1:17">
+      <c r="H109" s="31"/>
+      <c r="I109" s="31"/>
+    </row>
+    <row r="110" spans="1:17">
+      <c r="H110" s="31"/>
+      <c r="I110" s="31"/>
+    </row>
+    <row r="111" spans="1:17">
+      <c r="H111" s="31"/>
+      <c r="I111" s="31"/>
+    </row>
+    <row r="112" spans="1:17">
+      <c r="H112" s="31"/>
+      <c r="I112" s="31"/>
+    </row>
+    <row r="113" spans="8:9">
+      <c r="H113" s="31"/>
+      <c r="I113" s="31"/>
+    </row>
+    <row r="114" spans="8:9">
+      <c r="H114" s="31"/>
+      <c r="I114" s="31"/>
+    </row>
+    <row r="115" spans="8:9">
+      <c r="H115" s="31"/>
+      <c r="I115" s="31"/>
+    </row>
+    <row r="116" spans="8:9">
       <c r="H116" s="31"/>
       <c r="I116" s="31"/>
     </row>
-    <row r="117" spans="2:17">
+    <row r="117" spans="8:9">
       <c r="H117" s="31"/>
       <c r="I117" s="31"/>
     </row>
-    <row r="118" spans="2:17">
+    <row r="118" spans="8:9">
       <c r="H118" s="31"/>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="2:17">
+    <row r="119" spans="8:9">
       <c r="H119" s="31"/>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="2:17">
+    <row r="120" spans="8:9">
       <c r="H120" s="31"/>
       <c r="I120" s="31"/>
     </row>
-    <row r="121" spans="2:17">
+    <row r="121" spans="8:9">
       <c r="H121" s="31"/>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="2:17">
+    <row r="122" spans="8:9">
       <c r="H122" s="31"/>
       <c r="I122" s="31"/>
     </row>
-    <row r="123" spans="2:17">
+    <row r="123" spans="8:9">
       <c r="H123" s="31"/>
       <c r="I123" s="31"/>
     </row>
-    <row r="124" spans="2:17">
+    <row r="124" spans="8:9">
       <c r="H124" s="31"/>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="2:17">
+    <row r="125" spans="8:9">
       <c r="H125" s="31"/>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="2:17">
+    <row r="126" spans="8:9">
       <c r="H126" s="31"/>
       <c r="I126" s="31"/>
     </row>
-    <row r="127" spans="2:17">
+    <row r="127" spans="8:9">
       <c r="H127" s="31"/>
       <c r="I127" s="31"/>
     </row>
-    <row r="128" spans="2:17">
+    <row r="128" spans="8:9">
       <c r="H128" s="31"/>
       <c r="I128" s="31"/>
     </row>
@@ -10646,44 +10437,8 @@
       <c r="H222" s="31"/>
       <c r="I222" s="31"/>
     </row>
-    <row r="223" spans="8:9">
-      <c r="H223" s="31"/>
-      <c r="I223" s="31"/>
-    </row>
-    <row r="224" spans="8:9">
-      <c r="H224" s="31"/>
-      <c r="I224" s="31"/>
-    </row>
-    <row r="225" spans="8:9">
-      <c r="H225" s="31"/>
-      <c r="I225" s="31"/>
-    </row>
-    <row r="226" spans="8:9">
-      <c r="H226" s="31"/>
-      <c r="I226" s="31"/>
-    </row>
-    <row r="227" spans="8:9">
-      <c r="H227" s="31"/>
-      <c r="I227" s="31"/>
-    </row>
-    <row r="228" spans="8:9">
-      <c r="H228" s="31"/>
-      <c r="I228" s="31"/>
-    </row>
-    <row r="229" spans="8:9">
-      <c r="H229" s="31"/>
-      <c r="I229" s="31"/>
-    </row>
-    <row r="230" spans="8:9">
-      <c r="H230" s="31"/>
-      <c r="I230" s="31"/>
-    </row>
-    <row r="231" spans="8:9">
-      <c r="H231" s="31"/>
-      <c r="I231" s="31"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:Z158"/>
+  <autoFilter ref="A2:Z149"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>
@@ -10929,11 +10684,11 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="52" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="B8" s="52"/>
       <c r="C8" s="52" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="D8" s="52" t="s">
         <v>468</v>
@@ -10957,11 +10712,11 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="52" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="52" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>468</v>
@@ -10985,11 +10740,11 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="52" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="B10" s="52"/>
       <c r="C10" s="52" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="D10" s="52" t="s">
         <v>468</v>
@@ -11013,11 +10768,11 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="52" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="52" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="D11" s="52" t="s">
         <v>468</v>
@@ -11041,11 +10796,11 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="52" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="52" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="D12" s="52" t="s">
         <v>468</v>
@@ -11069,11 +10824,11 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="52" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="B13" s="52"/>
       <c r="C13" s="52" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="D13" s="52" t="s">
         <v>468</v>
@@ -11097,11 +10852,11 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="52" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
       <c r="B14" s="52"/>
       <c r="C14" s="52" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="D14" s="52" t="s">
         <v>468</v>
@@ -11125,11 +10880,11 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="52" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="B15" s="52"/>
       <c r="C15" s="52" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="D15" s="52" t="s">
         <v>468</v>
@@ -11153,11 +10908,11 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="52" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="B16" s="52"/>
       <c r="C16" s="52" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="D16" s="52" t="s">
         <v>468</v>
@@ -11181,11 +10936,11 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="52" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="B17" s="52"/>
       <c r="C17" s="52" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="D17" s="52" t="s">
         <v>468</v>
@@ -11209,11 +10964,11 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="52" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="B18" s="52"/>
       <c r="C18" s="52" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="D18" s="52" t="s">
         <v>468</v>
@@ -11237,11 +10992,11 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="52" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="B19" s="52"/>
       <c r="C19" s="52" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="D19" s="52" t="s">
         <v>468</v>
@@ -11265,11 +11020,11 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="52" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="B20" s="52"/>
       <c r="C20" s="52" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>468</v>
@@ -11293,11 +11048,11 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="52" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="B21" s="52"/>
       <c r="C21" s="52" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="D21" s="52" t="s">
         <v>468</v>
@@ -11321,14 +11076,14 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="52" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="B22" s="52"/>
       <c r="C22" s="52" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="D22" s="52" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="E22" s="52" t="s">
         <v>64</v>
@@ -11349,14 +11104,14 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="52" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="B23" s="52"/>
       <c r="C23" s="52" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="E23" s="52" t="s">
         <v>64</v>
@@ -11377,14 +11132,14 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="52" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="B24" s="52"/>
       <c r="C24" s="52" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="E24" s="52" t="s">
         <v>64</v>
@@ -11405,14 +11160,14 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="52" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="B25" s="52"/>
       <c r="C25" s="52" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="E25" s="52" t="s">
         <v>64</v>
@@ -11437,7 +11192,7 @@
       </c>
       <c r="B26" s="52"/>
       <c r="C26" s="52" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="D26" s="52" t="s">
         <v>707</v>
@@ -11465,7 +11220,7 @@
       </c>
       <c r="B27" s="52"/>
       <c r="C27" s="52" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="D27" s="52" t="s">
         <v>709</v>
@@ -11489,14 +11244,14 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="52" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="B28" s="52"/>
       <c r="C28" s="52" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="D28" s="52" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="E28" s="52" t="s">
         <v>64</v>
@@ -11519,14 +11274,14 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="52" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="B29" s="52"/>
       <c r="C29" s="52" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="E29" s="52" t="s">
         <v>64</v>
@@ -11549,14 +11304,14 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="52" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="B30" s="52"/>
       <c r="C30" s="52" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="E30" s="52" t="s">
         <v>64</v>
@@ -11579,14 +11334,14 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="52" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="B31" s="52"/>
       <c r="C31" s="52" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="D31" s="52" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="E31" s="52" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
fix hours not met metric
</commit_message>
<xml_diff>
--- a/projects/office_calibration_rgenoud_14_Sys3.xlsx
+++ b/projects/office_calibration_rgenoud_14_Sys3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="562" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2596,30 +2596,18 @@
     <t>Unmet Cooling Hours</t>
   </si>
   <si>
-    <t>standard_report.time_setpoint_not_met_during_occupied_cooling</t>
-  </si>
-  <si>
     <t>hrs</t>
   </si>
   <si>
     <t>Unmet Heating Hours</t>
   </si>
   <si>
-    <t>standard_report.time_setpoint_not_met_during_occupied_heating</t>
-  </si>
-  <si>
     <t>Total Unmet Hours</t>
   </si>
   <si>
-    <t>standard_report.time_setpoint_not_met_during_occupied_hours</t>
-  </si>
-  <si>
     <t>Building Area</t>
   </si>
   <si>
-    <t>standard_report.total_building_area</t>
-  </si>
-  <si>
     <t>m2</t>
   </si>
   <si>
@@ -2633,6 +2621,18 @@
   </si>
   <si>
     <t>wwr_multiplier</t>
+  </si>
+  <si>
+    <t>standard_reports.time_setpoint_not_met_during_occupied_cooling</t>
+  </si>
+  <si>
+    <t>standard_reports.time_setpoint_not_met_during_occupied_heating</t>
+  </si>
+  <si>
+    <t>standard_reports.time_setpoint_not_met_during_occupied_hours</t>
+  </si>
+  <si>
+    <t>standard_reports.total_building_area</t>
   </si>
 </sst>
 </file>
@@ -7474,7 +7474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
@@ -8898,13 +8898,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="48" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="E63" s="48" t="s">
         <v>68</v>
@@ -8915,10 +8915,10 @@
         <v>22</v>
       </c>
       <c r="D64" s="42" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="E64" s="42" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="F64" s="42" t="s">
         <v>64</v>
@@ -10456,9 +10456,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11079,11 +11079,11 @@
         <v>850</v>
       </c>
       <c r="B22" s="52"/>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="30" t="s">
+        <v>860</v>
+      </c>
+      <c r="D22" s="52" t="s">
         <v>851</v>
-      </c>
-      <c r="D22" s="52" t="s">
-        <v>852</v>
       </c>
       <c r="E22" s="52" t="s">
         <v>64</v>
@@ -11104,14 +11104,14 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="52" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B23" s="52"/>
-      <c r="C23" s="52" t="s">
-        <v>854</v>
+      <c r="C23" s="30" t="s">
+        <v>861</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E23" s="52" t="s">
         <v>64</v>
@@ -11132,14 +11132,14 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="52" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B24" s="52"/>
-      <c r="C24" s="52" t="s">
-        <v>856</v>
+      <c r="C24" s="30" t="s">
+        <v>862</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E24" s="52" t="s">
         <v>64</v>
@@ -11160,14 +11160,14 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="52" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="B25" s="52"/>
-      <c r="C25" s="52" t="s">
-        <v>858</v>
+      <c r="C25" s="30" t="s">
+        <v>863</v>
       </c>
       <c r="D25" s="52" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="E25" s="52" t="s">
         <v>64</v>

</xml_diff>